<commit_message>
workflow and excel updated
</commit_message>
<xml_diff>
--- a/data/excel/Blogs.xlsx
+++ b/data/excel/Blogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91846\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8555BE-F7ED-422E-87D6-48609B4E9E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A923DB7B-6A2E-4A83-81EC-974C5D6FFD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,7 +386,7 @@
 </t>
   </si>
   <si>
-    <t>Android 15: changes</t>
+    <t>Android</t>
   </si>
 </sst>
 </file>

</xml_diff>